<commit_message>
split screen and jump fix
</commit_message>
<xml_diff>
--- a/Metrics Data/Error Data.xlsx
+++ b/Metrics Data/Error Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Quality Assurance\SQA-Coursework\Metrics Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620BBFA-A583-44E0-819D-22E589B3BFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C67A2E0-A96A-4A6C-8DC5-BC8C5A2A5540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Data per C# File</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Double jump glitch</t>
+  </si>
+  <si>
+    <t>Milestone</t>
+  </si>
+  <si>
+    <t>TTO</t>
+  </si>
+  <si>
+    <t>ADMC</t>
+  </si>
+  <si>
+    <t>Player Controller</t>
   </si>
 </sst>
 </file>
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S5"/>
+  <dimension ref="B2:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,14 +421,15 @@
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="18" max="18" width="17.6640625" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -450,8 +463,17 @@
       <c r="S4" t="s">
         <v>13</v>
       </c>
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -484,6 +506,12 @@
       </c>
       <c r="S5">
         <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X5">
+        <v>-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>